<commit_message>
time series analysis with homelessness data
</commit_message>
<xml_diff>
--- a/Data/waiting_LQ_data.xlsx
+++ b/Data/waiting_LQ_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lokhe\Documents\year 3\ADS_year3_project_8\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linda\Documents\UNI\GitHub\ADS_year3_project_8\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF37C5AD-08DE-462C-827C-E3DFF8623368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D8F564-3D70-4C10-AB61-0A127979BE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{4BC8A5DB-25F5-4E61-B26C-E3F4C082ADEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{4BC8A5DB-25F5-4E61-B26C-E3F4C082ADEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>England</t>
   </si>
@@ -149,17 +151,26 @@
   <si>
     <t>price</t>
   </si>
+  <si>
+    <t>homeless</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="9">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot; &quot;#,##0&quot; &quot;;&quot;-&quot;#,##0&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
     <numFmt numFmtId="166" formatCode="0&quot; &quot;;&quot;-&quot;0&quot; &quot;"/>
+    <numFmt numFmtId="167" formatCode="&quot; &quot;General"/>
+    <numFmt numFmtId="176" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="177" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="178" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="179" formatCode="&quot; &quot;* #,##0.00&quot; &quot;;&quot;-&quot;* #,##0.00&quot; &quot;;&quot; &quot;* &quot;-&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="180" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +230,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +276,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -291,15 +340,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -362,13 +472,89 @@
     <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="6" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="6" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="57">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="8" xr:uid="{13873342-3218-4CCD-BF95-8B5DD0F90E84}"/>
+    <cellStyle name="Comma 2 2" xfId="9" xr:uid="{C9D78F43-214F-4E8A-BCB0-3B8F1CA44C2F}"/>
+    <cellStyle name="Comma 2 2 2" xfId="10" xr:uid="{09FE6D04-98B7-4CBC-8155-4F58CAA9F9A3}"/>
+    <cellStyle name="Comma 2 2 3 4" xfId="11" xr:uid="{A2FEE55F-0AD1-4162-8B76-A3F66C2869A6}"/>
+    <cellStyle name="Comma 2 3" xfId="12" xr:uid="{1966632A-07A1-4587-A8E1-9C31CCE65DBB}"/>
+    <cellStyle name="Comma 3" xfId="6" xr:uid="{0688813B-22DF-425F-8A47-91784E37FF0A}"/>
+    <cellStyle name="Comma 4" xfId="13" xr:uid="{79D8FFF3-17EC-40B0-9B44-76EA531D8B1B}"/>
+    <cellStyle name="Comma 5" xfId="14" xr:uid="{10389ADD-7B11-415A-8106-4C8F4D899866}"/>
+    <cellStyle name="Comma 7 2" xfId="15" xr:uid="{491ABB67-C242-4A0E-89BA-DE1E1CDACD7E}"/>
+    <cellStyle name="Comma 7 2 2" xfId="16" xr:uid="{EEC8E31D-EB99-4EDF-8043-1BF05020D6E1}"/>
+    <cellStyle name="Hyperlink" xfId="17" xr:uid="{18D216AD-FF15-48B6-A32E-21F7BF2D8986}"/>
+    <cellStyle name="Hyperlink 2" xfId="18" xr:uid="{327B8C8C-E4A5-43BD-A243-F59A3C5FD5F1}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="19" xr:uid="{4D86D1A5-BEDD-4522-94C2-9CC7B5EC517C}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 11" xfId="20" xr:uid="{3C2DF0C4-709B-4FDF-ABE2-9B3F44BEA78A}"/>
+    <cellStyle name="Normal 13" xfId="21" xr:uid="{4394DC33-196F-42D2-882E-52DFD14D88D9}"/>
+    <cellStyle name="Normal 13 2" xfId="22" xr:uid="{61737A69-4C9C-4B4C-ADC2-CCA6CBA4C5FF}"/>
+    <cellStyle name="Normal 13 2 2" xfId="23" xr:uid="{DEE24093-16FA-4EB9-B70F-37E8649E3F46}"/>
+    <cellStyle name="Normal 13 3" xfId="24" xr:uid="{4CA9AB65-E7FD-4570-909F-B8F190698B75}"/>
+    <cellStyle name="Normal 13 3 2" xfId="25" xr:uid="{3B311A53-EACC-49A4-A7DE-9108226DB3DC}"/>
+    <cellStyle name="Normal 13 3 2 2" xfId="26" xr:uid="{3E0553CF-4817-4E70-AD77-77FA6386A05F}"/>
+    <cellStyle name="Normal 13 4" xfId="27" xr:uid="{DBA9DA94-5634-4E5A-8FD5-AE28F1DD6600}"/>
+    <cellStyle name="Normal 13 5" xfId="28" xr:uid="{B6B5B820-A8B3-45F1-8729-9A7D92A5E958}"/>
+    <cellStyle name="Normal 2" xfId="29" xr:uid="{BDACDE58-91DA-4092-A54D-E432BA8D3AEE}"/>
+    <cellStyle name="Normal 2 3 2" xfId="30" xr:uid="{C5C26AD8-64E5-448A-8461-FF045A2C6D5B}"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="31" xr:uid="{16564F4F-EB27-4F0A-AE98-C2002A5CA62E}"/>
+    <cellStyle name="Normal 2 3 3" xfId="32" xr:uid="{5CEB110E-7BCA-48AD-8053-1222C55FFC96}"/>
     <cellStyle name="Normal 2 8" xfId="4" xr:uid="{A4EA2D9B-CBAF-4759-B81F-CAA9F1BD4559}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{BC11C541-586A-47C1-BF14-48211653C68E}"/>
     <cellStyle name="Normal 3 2" xfId="2" xr:uid="{6CBEB49A-4C70-4759-A19B-5AD74F1B81B7}"/>
+    <cellStyle name="Normal 3 2 2" xfId="34" xr:uid="{F26A2D49-5FC2-446C-85B3-5A1EB9F87A20}"/>
+    <cellStyle name="Normal 3 3" xfId="33" xr:uid="{1795687C-86E5-4313-B37E-4C4292A00F0B}"/>
+    <cellStyle name="Normal 3 4" xfId="35" xr:uid="{22217BE7-8F87-4311-A5C4-7CCE22E7B7A8}"/>
+    <cellStyle name="Normal 4" xfId="36" xr:uid="{5982A503-1DB7-4A84-ABB9-BEAE517E45C2}"/>
+    <cellStyle name="Normal 5" xfId="37" xr:uid="{022F1AAF-EE48-4CB7-88C3-60F52F685933}"/>
+    <cellStyle name="Normal 5 2" xfId="38" xr:uid="{F4F1A2EC-98F1-46F8-9713-FF61C38380A5}"/>
+    <cellStyle name="Normal 6" xfId="39" xr:uid="{3B56FA4A-CD3D-42E8-B9F1-EE5F07DE475A}"/>
+    <cellStyle name="Normal 6 2" xfId="40" xr:uid="{FD5B0243-BD5A-422F-AFB1-53A2CE3BB7CB}"/>
+    <cellStyle name="Normal 7" xfId="41" xr:uid="{AB98D910-CC0A-4394-80E0-343FF9FD179D}"/>
+    <cellStyle name="Normal 7 2" xfId="42" xr:uid="{B750CFEE-1F74-46B1-902F-07FAEDD3C845}"/>
+    <cellStyle name="Normal 8" xfId="43" xr:uid="{97EBED6D-50D2-48CB-8BDC-204A57C5A037}"/>
+    <cellStyle name="Normal 8 2" xfId="44" xr:uid="{C90EBDB3-DFFE-401F-A101-650A8FE2CF7E}"/>
+    <cellStyle name="Normal 9" xfId="5" xr:uid="{6216E0B1-D508-4442-A292-C8A70921F8B3}"/>
+    <cellStyle name="Normal_TABLE1 0609" xfId="45" xr:uid="{4EC821E4-94AD-450F-89FC-7D68D39EA3D4}"/>
+    <cellStyle name="Percent 10 2" xfId="46" xr:uid="{821D2432-9435-4BCF-A30F-6B7C2099119D}"/>
+    <cellStyle name="Percent 2" xfId="47" xr:uid="{66A321B3-6111-4178-A649-69535C99EC7E}"/>
+    <cellStyle name="Percent 2 2" xfId="48" xr:uid="{042EB196-88A3-4957-8082-8B020C936306}"/>
+    <cellStyle name="Percent 2 3" xfId="49" xr:uid="{A7F0962F-051E-49CF-A4DF-6668BA1FB7C6}"/>
+    <cellStyle name="Percent 2 3 2 2" xfId="50" xr:uid="{70151F5C-2B71-422D-BA75-20DD0E2E5EC7}"/>
+    <cellStyle name="Percent 2 3 3" xfId="51" xr:uid="{405D914D-CC39-43AC-B99B-8FEC566BD692}"/>
+    <cellStyle name="Percent 2 4" xfId="52" xr:uid="{4EBDB59F-E6E8-411D-BC43-F15434982678}"/>
+    <cellStyle name="Percent 2 4 2" xfId="53" xr:uid="{BAE9716E-CCB2-46CD-B88E-4FF79B80E198}"/>
+    <cellStyle name="Percent 3" xfId="7" xr:uid="{C1A60007-9001-4C8D-8270-3787525DDE15}"/>
+    <cellStyle name="Percent 3 2" xfId="54" xr:uid="{9C4266CA-00C1-463E-AF52-EDC3966063D3}"/>
+    <cellStyle name="Percent 8" xfId="55" xr:uid="{0B5B9F65-D2FC-4067-967B-F684612B974D}"/>
+    <cellStyle name="Percent 9 2" xfId="56" xr:uid="{250031F0-CDEC-474F-B706-7C8785709AE8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -682,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084147DA-F94D-4870-8757-C08495B57EE9}">
   <dimension ref="A1:AL12"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:AK3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1947,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDC2EA0-D6FF-41DE-AB22-BB51443BB077}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:U3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4542,8 +4728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3ECB9A-13FE-4C2B-B2A8-3180F39BF7D2}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4558,6 +4744,9 @@
       <c r="C1" t="s">
         <v>35</v>
       </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
@@ -4569,7 +4758,9 @@
       <c r="C2" s="16">
         <v>67000</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="32">
+        <v>123840</v>
+      </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -4598,7 +4789,9 @@
       <c r="C3" s="16">
         <v>80000</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="32">
+        <v>135580</v>
+      </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -4627,7 +4820,9 @@
       <c r="C4" s="16">
         <v>100000</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="32">
+        <v>127750</v>
+      </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -4656,7 +4851,9 @@
       <c r="C5" s="16">
         <v>112500</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="32">
+        <v>100170</v>
+      </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
@@ -4685,7 +4882,9 @@
       <c r="C6" s="16">
         <v>119995</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="32">
+        <v>76860</v>
+      </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -4714,7 +4913,9 @@
       <c r="C7" s="16">
         <v>125000</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="32">
+        <v>64970</v>
+      </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -4743,7 +4944,9 @@
       <c r="C8" s="16">
         <v>125000</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="32">
+        <v>57510</v>
+      </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -4772,7 +4975,9 @@
       <c r="C9" s="16">
         <v>120000</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="32">
+        <v>41780</v>
+      </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
@@ -4801,7 +5006,9 @@
       <c r="C10" s="16">
         <v>127500</v>
       </c>
-      <c r="D10" s="16"/>
+      <c r="D10" s="32">
+        <v>42390</v>
+      </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -4830,7 +5037,9 @@
       <c r="C11" s="16">
         <v>125000</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="32">
+        <v>48510</v>
+      </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -4859,7 +5068,9 @@
       <c r="C12" s="16">
         <v>125000</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="33">
+        <v>53480</v>
+      </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -4888,7 +5099,9 @@
       <c r="C13" s="16">
         <v>127000</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="32">
+        <v>53210</v>
+      </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -4917,7 +5130,9 @@
       <c r="C14" s="16">
         <v>134000</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="32">
+        <v>53410</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -4946,7 +5161,9 @@
       <c r="C15" s="16">
         <v>139950</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="32">
+        <v>56500</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -4975,7 +5192,9 @@
       <c r="C16" s="16">
         <v>145000</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="32">
+        <v>59260</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -5004,7 +5223,9 @@
       <c r="C17" s="16">
         <v>150000</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="34">
+        <v>57890</v>
+      </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -5033,7 +5254,9 @@
       <c r="C18" s="16">
         <v>156000</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="32">
+        <v>35770</v>
+      </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -5062,7 +5285,9 @@
       <c r="C19" s="16">
         <v>160000</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="32">
+        <v>37830</v>
+      </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
@@ -5091,7 +5316,9 @@
       <c r="C20" s="16">
         <v>164000</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="32">
+        <v>40300</v>
+      </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
@@ -5117,4 +5344,452 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48712ED-A58E-4EBF-BDEC-09018F5EAADC}">
+  <dimension ref="A2:Y3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:25" ht="40" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1998</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1999</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="8">
+        <v>2001</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2002</v>
+      </c>
+      <c r="H2" s="8">
+        <v>2003</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2004</v>
+      </c>
+      <c r="J2" s="8">
+        <v>2005</v>
+      </c>
+      <c r="K2" s="8">
+        <v>2006</v>
+      </c>
+      <c r="L2" s="8">
+        <v>2007</v>
+      </c>
+      <c r="M2" s="8">
+        <v>2008</v>
+      </c>
+      <c r="N2" s="8">
+        <v>2009</v>
+      </c>
+      <c r="O2" s="8">
+        <v>2010</v>
+      </c>
+      <c r="P2" s="8">
+        <v>2011</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>2012</v>
+      </c>
+      <c r="R2" s="8">
+        <v>2013</v>
+      </c>
+      <c r="S2" s="8">
+        <v>2014</v>
+      </c>
+      <c r="T2" s="8">
+        <v>2015</v>
+      </c>
+      <c r="U2" s="8">
+        <v>2016</v>
+      </c>
+      <c r="V2" s="8">
+        <v>2017</v>
+      </c>
+      <c r="W2" s="8">
+        <v>2018</v>
+      </c>
+      <c r="X2" s="8">
+        <v>2019</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="37">
+        <v>104630</v>
+      </c>
+      <c r="D3" s="37">
+        <v>105380</v>
+      </c>
+      <c r="E3" s="37">
+        <v>111340</v>
+      </c>
+      <c r="F3" s="37">
+        <v>117820</v>
+      </c>
+      <c r="G3" s="37">
+        <v>123840</v>
+      </c>
+      <c r="H3" s="37">
+        <v>135580</v>
+      </c>
+      <c r="I3" s="37">
+        <v>127750</v>
+      </c>
+      <c r="J3" s="37">
+        <v>100170</v>
+      </c>
+      <c r="K3" s="37">
+        <v>76860</v>
+      </c>
+      <c r="L3" s="37">
+        <v>64970</v>
+      </c>
+      <c r="M3" s="37">
+        <v>57510</v>
+      </c>
+      <c r="N3" s="37">
+        <v>41780</v>
+      </c>
+      <c r="O3" s="37">
+        <v>42390</v>
+      </c>
+      <c r="P3" s="37">
+        <v>48510</v>
+      </c>
+      <c r="Q3" s="38">
+        <v>53480</v>
+      </c>
+      <c r="R3" s="37">
+        <v>53210</v>
+      </c>
+      <c r="S3" s="37">
+        <v>53410</v>
+      </c>
+      <c r="T3" s="37">
+        <v>56500</v>
+      </c>
+      <c r="U3" s="37">
+        <v>59260</v>
+      </c>
+      <c r="V3" s="39">
+        <v>57890</v>
+      </c>
+      <c r="W3" s="37">
+        <v>35770</v>
+      </c>
+      <c r="X3" s="37">
+        <v>37830</v>
+      </c>
+      <c r="Y3" s="37">
+        <v>40300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E6DAE1-36CB-4643-B4B5-A07F7929B1A0}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1998</v>
+      </c>
+      <c r="B2" s="35">
+        <v>1020229</v>
+      </c>
+      <c r="C2" s="37">
+        <v>104630</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1999</v>
+      </c>
+      <c r="B3" s="35">
+        <v>1036751</v>
+      </c>
+      <c r="C3" s="37">
+        <v>105380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="35">
+        <v>1038720</v>
+      </c>
+      <c r="C4" s="37">
+        <v>111340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2001</v>
+      </c>
+      <c r="B5" s="35">
+        <v>1039265</v>
+      </c>
+      <c r="C5" s="37">
+        <v>117820</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2002</v>
+      </c>
+      <c r="B6" s="35">
+        <v>1093342</v>
+      </c>
+      <c r="C6" s="37">
+        <v>123840</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2003</v>
+      </c>
+      <c r="B7" s="35">
+        <v>1263931</v>
+      </c>
+      <c r="C7" s="37">
+        <v>135580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2004</v>
+      </c>
+      <c r="B8" s="35">
+        <v>1434874</v>
+      </c>
+      <c r="C8" s="37">
+        <v>127750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2005</v>
+      </c>
+      <c r="B9" s="35">
+        <v>1543337</v>
+      </c>
+      <c r="C9" s="37">
+        <v>100170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10" s="35">
+        <v>1634301</v>
+      </c>
+      <c r="C10" s="37">
+        <v>76860</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2007</v>
+      </c>
+      <c r="B11" s="35">
+        <v>1674421</v>
+      </c>
+      <c r="C11" s="37">
+        <v>64970</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2008</v>
+      </c>
+      <c r="B12" s="35">
+        <v>1769939</v>
+      </c>
+      <c r="C12" s="37">
+        <v>57510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2009</v>
+      </c>
+      <c r="B13" s="35">
+        <v>1763140</v>
+      </c>
+      <c r="C13" s="37">
+        <v>41780</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="35">
+        <v>1740997</v>
+      </c>
+      <c r="C14" s="37">
+        <v>42390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="35">
+        <v>1813559</v>
+      </c>
+      <c r="C15" s="37">
+        <v>48510</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="B16" s="36">
+        <v>1850929</v>
+      </c>
+      <c r="C16" s="38">
+        <v>53480</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17" s="36">
+        <v>1685814</v>
+      </c>
+      <c r="C17" s="37">
+        <v>53210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18" s="36">
+        <v>1368312</v>
+      </c>
+      <c r="C18" s="37">
+        <v>53410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2015</v>
+      </c>
+      <c r="B19" s="36">
+        <v>1255613</v>
+      </c>
+      <c r="C19" s="37">
+        <v>56500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2016</v>
+      </c>
+      <c r="B20" s="36">
+        <v>1183779</v>
+      </c>
+      <c r="C20" s="37">
+        <v>59260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2017</v>
+      </c>
+      <c r="B21" s="36">
+        <v>1157044</v>
+      </c>
+      <c r="C21" s="39">
+        <v>57890</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2018</v>
+      </c>
+      <c r="B22" s="36">
+        <v>1115285</v>
+      </c>
+      <c r="C22" s="37">
+        <v>35770</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2019</v>
+      </c>
+      <c r="B23" s="36">
+        <v>1159833</v>
+      </c>
+      <c r="C23" s="37">
+        <v>37830</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2020</v>
+      </c>
+      <c r="B24" s="36">
+        <v>1145501</v>
+      </c>
+      <c r="C24" s="37">
+        <v>40300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add more pearson r calcs
</commit_message>
<xml_diff>
--- a/Data/waiting_LQ_data.xlsx
+++ b/Data/waiting_LQ_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linda\Documents\UNI\GitHub\ADS_year3_project_8\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lokhe\Documents\year 3\ADS_year3_project_8\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D8F564-3D70-4C10-AB61-0A127979BE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9080CFD2-F90D-4AAB-A8D4-CB40102DE6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{4BC8A5DB-25F5-4E61-B26C-E3F4C082ADEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{4BC8A5DB-25F5-4E61-B26C-E3F4C082ADEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="39">
   <si>
     <t>England</t>
   </si>
@@ -154,21 +154,27 @@
   <si>
     <t>homeless</t>
   </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>earning</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot; &quot;#,##0&quot; &quot;;&quot;-&quot;#,##0&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
-    <numFmt numFmtId="166" formatCode="0&quot; &quot;;&quot;-&quot;0&quot; &quot;"/>
-    <numFmt numFmtId="167" formatCode="&quot; &quot;General"/>
-    <numFmt numFmtId="176" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
-    <numFmt numFmtId="177" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
-    <numFmt numFmtId="178" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
-    <numFmt numFmtId="179" formatCode="&quot; &quot;* #,##0.00&quot; &quot;;&quot;-&quot;* #,##0.00&quot; &quot;;&quot; &quot;* &quot;-&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
-    <numFmt numFmtId="180" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot; &quot;#,##0&quot; &quot;;&quot;-&quot;#,##0&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="165" formatCode="0&quot; &quot;;&quot;-&quot;0&quot; &quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot; &quot;General"/>
+    <numFmt numFmtId="167" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="170" formatCode="&quot; &quot;* #,##0.00&quot; &quot;;&quot;-&quot;* #,##0.00&quot; &quot;;&quot; &quot;* &quot;-&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="171" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -352,22 +358,22 @@
   </borders>
   <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -386,7 +392,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
@@ -396,7 +402,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,7 +422,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -432,7 +438,7 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -483,7 +489,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2134,7 +2140,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2998,8 +3004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE08E4B-FABB-44B6-930F-80E5889639C2}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4728,8 +4734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3ECB9A-13FE-4C2B-B2A8-3180F39BF7D2}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4747,6 +4753,12 @@
       <c r="D1" t="s">
         <v>36</v>
       </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
@@ -4761,8 +4773,12 @@
       <c r="D2" s="32">
         <v>123840</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="28">
+        <v>4.41</v>
+      </c>
+      <c r="F2" s="22">
+        <v>14755</v>
+      </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
@@ -4792,8 +4808,12 @@
       <c r="D3" s="32">
         <v>135580</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="E3" s="28">
+        <v>5.17</v>
+      </c>
+      <c r="F3" s="22">
+        <v>15293</v>
+      </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -4823,8 +4843,12 @@
       <c r="D4" s="32">
         <v>127750</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="E4" s="28">
+        <v>6.16</v>
+      </c>
+      <c r="F4" s="22">
+        <v>15909</v>
+      </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -4854,8 +4878,12 @@
       <c r="D5" s="32">
         <v>100170</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="28">
+        <v>6.7</v>
+      </c>
+      <c r="F5" s="22">
+        <v>16427</v>
+      </c>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -4885,8 +4913,12 @@
       <c r="D6" s="32">
         <v>76860</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="28">
+        <v>7.15</v>
+      </c>
+      <c r="F6" s="22">
+        <v>16645</v>
+      </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -4916,8 +4948,12 @@
       <c r="D7" s="32">
         <v>64970</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="28">
+        <v>7.26</v>
+      </c>
+      <c r="F7" s="22">
+        <v>17227</v>
+      </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
@@ -4947,8 +4983,12 @@
       <c r="D8" s="32">
         <v>57510</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="28">
+        <v>6.96</v>
+      </c>
+      <c r="F8" s="22">
+        <v>17968</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
@@ -4978,8 +5018,12 @@
       <c r="D9" s="32">
         <v>41780</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="E9" s="28">
+        <v>6.41</v>
+      </c>
+      <c r="F9" s="22">
+        <v>18395</v>
+      </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -5009,8 +5053,12 @@
       <c r="D10" s="32">
         <v>42390</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="E10" s="28">
+        <v>6.76</v>
+      </c>
+      <c r="F10" s="22">
+        <v>18495</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
@@ -5040,8 +5088,12 @@
       <c r="D11" s="32">
         <v>48510</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="E11" s="28">
+        <v>6.64</v>
+      </c>
+      <c r="F11" s="22">
+        <v>18528</v>
+      </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -5071,8 +5123,12 @@
       <c r="D12" s="33">
         <v>53480</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="28">
+        <v>6.61</v>
+      </c>
+      <c r="F12" s="22">
+        <v>18920</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -5102,8 +5158,12 @@
       <c r="D13" s="32">
         <v>53210</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="E13" s="28">
+        <v>6.51</v>
+      </c>
+      <c r="F13" s="22">
+        <v>19215</v>
+      </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -5133,8 +5193,12 @@
       <c r="D14" s="32">
         <v>53410</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="28">
+        <v>6.73</v>
+      </c>
+      <c r="F14" s="22">
+        <v>19317</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
@@ -5164,8 +5228,12 @@
       <c r="D15" s="32">
         <v>56500</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="E15" s="28">
+        <v>6.94</v>
+      </c>
+      <c r="F15" s="22">
+        <v>19583</v>
+      </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -5195,8 +5263,12 @@
       <c r="D16" s="32">
         <v>59260</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="28">
+        <v>7.05</v>
+      </c>
+      <c r="F16" s="22">
+        <v>20141</v>
+      </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -5226,8 +5298,12 @@
       <c r="D17" s="34">
         <v>57890</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="E17" s="28">
+        <v>7.15</v>
+      </c>
+      <c r="F17" s="22">
+        <v>20569</v>
+      </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
@@ -5257,8 +5333,12 @@
       <c r="D18" s="32">
         <v>35770</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="28">
+        <v>7.18</v>
+      </c>
+      <c r="F18" s="22">
+        <v>21165</v>
+      </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
@@ -5288,8 +5368,12 @@
       <c r="D19" s="32">
         <v>37830</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="E19" s="28">
+        <v>7.05</v>
+      </c>
+      <c r="F19" s="16">
+        <v>21985</v>
+      </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -5319,8 +5403,12 @@
       <c r="D20" s="32">
         <v>40300</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="E20" s="15">
+        <v>7.01</v>
+      </c>
+      <c r="F20" s="16">
+        <v>22813</v>
+      </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
@@ -5350,7 +5438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48712ED-A58E-4EBF-BDEC-09018F5EAADC}">
   <dimension ref="A2:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -5519,7 +5607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E6DAE1-36CB-4643-B4B5-A07F7929B1A0}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more correlation but nothing is correlating
</commit_message>
<xml_diff>
--- a/Data/waiting_LQ_data.xlsx
+++ b/Data/waiting_LQ_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lokhe\Documents\year 3\ADS_year3_project_8\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9080CFD2-F90D-4AAB-A8D4-CB40102DE6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F451520A-3657-4719-A578-FA47FE92E437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{4BC8A5DB-25F5-4E61-B26C-E3F4C082ADEE}"/>
   </bookViews>
@@ -20,6 +20,8 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>England</t>
   </si>
@@ -160,12 +162,27 @@
   <si>
     <t>earning</t>
   </si>
+  <si>
+    <t>householdPop</t>
+  </si>
+  <si>
+    <t>household population</t>
+  </si>
+  <si>
+    <t>affordable completed</t>
+  </si>
+  <si>
+    <t>social rent lettings</t>
+  </si>
+  <si>
+    <t>social Lettings</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="11">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot; &quot;#,##0&quot; &quot;;&quot;-&quot;#,##0&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
     <numFmt numFmtId="165" formatCode="0&quot; &quot;;&quot;-&quot;0&quot; &quot;"/>
@@ -175,8 +192,10 @@
     <numFmt numFmtId="169" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
     <numFmt numFmtId="170" formatCode="&quot; &quot;* #,##0.00&quot; &quot;;&quot;-&quot;* #,##0.00&quot; &quot;;&quot; &quot;* &quot;-&quot;#&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
     <numFmt numFmtId="171" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +286,17 @@
       <color rgb="FF000000"/>
       <name val="Courier"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -415,7 +445,7 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -501,6 +531,22 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="6" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="14" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="14" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="15" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -4735,12 +4781,14 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
@@ -4759,6 +4807,15 @@
       <c r="F1" t="s">
         <v>38</v>
       </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
@@ -4779,7 +4836,9 @@
       <c r="F2" s="22">
         <v>14755</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="40">
+        <v>20553236</v>
+      </c>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
@@ -4814,7 +4873,9 @@
       <c r="F3" s="22">
         <v>15293</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="40">
+        <v>20650943</v>
+      </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -4849,7 +4910,9 @@
       <c r="F4" s="22">
         <v>15909</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="40">
+        <v>20751955</v>
+      </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
@@ -4884,7 +4947,9 @@
       <c r="F5" s="22">
         <v>16427</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="40">
+        <v>20925683</v>
+      </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
@@ -4919,7 +4984,9 @@
       <c r="F6" s="22">
         <v>16645</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="40">
+        <v>21071616</v>
+      </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -4954,9 +5021,13 @@
       <c r="F7" s="22">
         <v>17227</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="40">
+        <v>21223341</v>
+      </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="I7" s="43">
+        <v>366820</v>
+      </c>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
@@ -4989,9 +5060,13 @@
       <c r="F8" s="22">
         <v>17968</v>
       </c>
-      <c r="G8" s="16"/>
+      <c r="G8" s="40">
+        <v>21399891</v>
+      </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="I8" s="43">
+        <v>379082</v>
+      </c>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
@@ -5024,9 +5099,15 @@
       <c r="F9" s="22">
         <v>18395</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
+      <c r="G9" s="40">
+        <v>21561859</v>
+      </c>
+      <c r="H9" s="42">
+        <v>40550</v>
+      </c>
+      <c r="I9" s="43">
+        <v>367755</v>
+      </c>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
@@ -5059,9 +5140,15 @@
       <c r="F10" s="22">
         <v>18495</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="G10" s="40">
+        <v>21742577</v>
+      </c>
+      <c r="H10" s="42">
+        <v>43040</v>
+      </c>
+      <c r="I10" s="43">
+        <v>393625</v>
+      </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
@@ -5094,9 +5181,15 @@
       <c r="F11" s="22">
         <v>18528</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
+      <c r="G11" s="40">
+        <v>21976219</v>
+      </c>
+      <c r="H11" s="42">
+        <v>35558</v>
+      </c>
+      <c r="I11" s="43">
+        <v>389805</v>
+      </c>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
@@ -5129,9 +5222,15 @@
       <c r="F12" s="22">
         <v>18920</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="G12" s="40">
+        <v>22130484</v>
+      </c>
+      <c r="H12" s="42">
+        <v>28600</v>
+      </c>
+      <c r="I12" s="43">
+        <v>350135</v>
+      </c>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
@@ -5164,9 +5263,15 @@
       <c r="F13" s="22">
         <v>19215</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="G13" s="40">
+        <v>22291124</v>
+      </c>
+      <c r="H13" s="42">
+        <v>27606</v>
+      </c>
+      <c r="I13" s="43">
+        <v>359077</v>
+      </c>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
@@ -5199,9 +5304,15 @@
       <c r="F14" s="22">
         <v>19317</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="G14" s="40">
+        <v>22487754</v>
+      </c>
+      <c r="H14" s="42">
+        <v>40864</v>
+      </c>
+      <c r="I14" s="43">
+        <v>345279</v>
+      </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
@@ -5234,9 +5345,15 @@
       <c r="F15" s="22">
         <v>19583</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="G15" s="40">
+        <v>22681178</v>
+      </c>
+      <c r="H15" s="42">
+        <v>17390</v>
+      </c>
+      <c r="I15" s="43">
+        <v>327448.30018399446</v>
+      </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
@@ -5269,9 +5386,15 @@
       <c r="F16" s="22">
         <v>20141</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
+      <c r="G16" s="40">
+        <v>22884180</v>
+      </c>
+      <c r="H16" s="42">
+        <v>22885</v>
+      </c>
+      <c r="I16" s="43">
+        <v>290060.03519140871</v>
+      </c>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
@@ -5304,9 +5427,15 @@
       <c r="F17" s="22">
         <v>20569</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
+      <c r="G17" s="40">
+        <v>23047198</v>
+      </c>
+      <c r="H17" s="42">
+        <v>25862</v>
+      </c>
+      <c r="I17" s="43">
+        <v>272805.656815511</v>
+      </c>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
@@ -5339,9 +5468,15 @@
       <c r="F18" s="22">
         <v>21165</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
+      <c r="G18" s="40">
+        <v>23204246</v>
+      </c>
+      <c r="H18" s="42">
+        <v>28716</v>
+      </c>
+      <c r="I18" s="44">
+        <v>272829.93613078265</v>
+      </c>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
@@ -5375,8 +5510,12 @@
         <v>21985</v>
       </c>
       <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
+      <c r="H19" s="42">
+        <v>28226</v>
+      </c>
+      <c r="I19" s="44">
+        <v>264239.22071551759</v>
+      </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
@@ -5410,7 +5549,9 @@
         <v>22813</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="H20" s="42">
+        <v>24002</v>
+      </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
@@ -5428,9 +5569,13 @@
     <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="9"/>
       <c r="B21" s="4"/>
+      <c r="H21" s="42">
+        <v>10007</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5608,7 +5753,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C24"/>
+      <selection activeCell="A11" sqref="A11:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5880,4 +6025,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C132130-043A-46F6-8E3F-6001DEB15A0E}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="41">
+        <v>2002</v>
+      </c>
+      <c r="B2" s="41">
+        <v>2003</v>
+      </c>
+      <c r="C2" s="41">
+        <v>2004</v>
+      </c>
+      <c r="D2" s="41">
+        <v>2005</v>
+      </c>
+      <c r="E2" s="41">
+        <v>2006</v>
+      </c>
+      <c r="F2" s="41">
+        <v>2007</v>
+      </c>
+      <c r="G2" s="41">
+        <v>2008</v>
+      </c>
+      <c r="H2" s="41">
+        <v>2009</v>
+      </c>
+      <c r="I2" s="41">
+        <v>2010</v>
+      </c>
+      <c r="J2" s="41">
+        <v>2011</v>
+      </c>
+      <c r="K2" s="41">
+        <v>2012</v>
+      </c>
+      <c r="L2" s="41">
+        <v>2013</v>
+      </c>
+      <c r="M2" s="41">
+        <v>2014</v>
+      </c>
+      <c r="N2" s="41">
+        <v>2015</v>
+      </c>
+      <c r="O2" s="41">
+        <v>2016</v>
+      </c>
+      <c r="P2" s="41">
+        <v>2017</v>
+      </c>
+      <c r="Q2" s="41">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="40">
+        <v>20553236</v>
+      </c>
+      <c r="B3" s="40">
+        <v>20650943</v>
+      </c>
+      <c r="C3" s="40">
+        <v>20751955</v>
+      </c>
+      <c r="D3" s="40">
+        <v>20925683</v>
+      </c>
+      <c r="E3" s="40">
+        <v>21071616</v>
+      </c>
+      <c r="F3" s="40">
+        <v>21223341</v>
+      </c>
+      <c r="G3" s="40">
+        <v>21399891</v>
+      </c>
+      <c r="H3" s="40">
+        <v>21561859</v>
+      </c>
+      <c r="I3" s="40">
+        <v>21742577</v>
+      </c>
+      <c r="J3" s="40">
+        <v>21976219</v>
+      </c>
+      <c r="K3" s="40">
+        <v>22130484</v>
+      </c>
+      <c r="L3" s="40">
+        <v>22291124</v>
+      </c>
+      <c r="M3" s="40">
+        <v>22487754</v>
+      </c>
+      <c r="N3" s="40">
+        <v>22681178</v>
+      </c>
+      <c r="O3" s="40">
+        <v>22884180</v>
+      </c>
+      <c r="P3" s="40">
+        <v>23047198</v>
+      </c>
+      <c r="Q3" s="40">
+        <v>23204246</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77CC801-B672-4F72-8810-CE985DDD8ADB}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2007</v>
+      </c>
+      <c r="B2">
+        <v>2008</v>
+      </c>
+      <c r="C2">
+        <v>2009</v>
+      </c>
+      <c r="D2">
+        <v>2010</v>
+      </c>
+      <c r="E2">
+        <v>2011</v>
+      </c>
+      <c r="F2">
+        <v>2012</v>
+      </c>
+      <c r="G2">
+        <v>2013</v>
+      </c>
+      <c r="H2">
+        <v>2014</v>
+      </c>
+      <c r="I2">
+        <v>2015</v>
+      </c>
+      <c r="J2">
+        <v>2016</v>
+      </c>
+      <c r="K2">
+        <v>2017</v>
+      </c>
+      <c r="L2">
+        <v>2018</v>
+      </c>
+      <c r="M2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="43">
+        <v>366820</v>
+      </c>
+      <c r="B3" s="43">
+        <v>379082</v>
+      </c>
+      <c r="C3" s="43">
+        <v>367755</v>
+      </c>
+      <c r="D3" s="43">
+        <v>393625</v>
+      </c>
+      <c r="E3" s="43">
+        <v>389805</v>
+      </c>
+      <c r="F3" s="43">
+        <v>350135</v>
+      </c>
+      <c r="G3" s="43">
+        <v>359077</v>
+      </c>
+      <c r="H3" s="43">
+        <v>345279</v>
+      </c>
+      <c r="I3" s="43">
+        <v>327448.30018399446</v>
+      </c>
+      <c r="J3" s="43">
+        <v>290060.03519140871</v>
+      </c>
+      <c r="K3" s="43">
+        <v>272805.656815511</v>
+      </c>
+      <c r="L3" s="44">
+        <v>272829.93613078265</v>
+      </c>
+      <c r="M3" s="44">
+        <v>264239.22071551759</v>
+      </c>
+      <c r="O3" s="45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>